<commit_message>
payment page models fix
</commit_message>
<xml_diff>
--- a/cypress/fixtures/b2c/flightDetails.xlsx
+++ b/cypress/fixtures/b2c/flightDetails.xlsx
@@ -90,9 +90,6 @@
     <t>Promo Code</t>
   </si>
   <si>
-    <t>TC001</t>
-  </si>
-  <si>
     <t>DXB</t>
   </si>
   <si>
@@ -123,9 +120,6 @@
     <t>IT000@2</t>
   </si>
   <si>
-    <t>TC002</t>
-  </si>
-  <si>
     <t>AUH</t>
   </si>
   <si>
@@ -142,9 +136,6 @@
   </si>
   <si>
     <t>Etihad Airways</t>
-  </si>
-  <si>
-    <t>TC003</t>
   </si>
   <si>
     <t>DOH</t>
@@ -168,9 +159,6 @@
     <t>Qatar Airways</t>
   </si>
   <si>
-    <t>TC004</t>
-  </si>
-  <si>
     <t>BOM</t>
   </si>
   <si>
@@ -187,9 +175,6 @@
   </si>
   <si>
     <t>Non Refundable</t>
-  </si>
-  <si>
-    <t>TC005</t>
   </si>
   <si>
     <t>CAI</t>
@@ -216,13 +201,7 @@
     <t>Egyptair</t>
   </si>
   <si>
-    <t>TC006</t>
-  </si>
-  <si>
     <t>AE</t>
-  </si>
-  <si>
-    <t>TC007</t>
   </si>
   <si>
     <t>JED</t>
@@ -240,16 +219,10 @@
     <t>Saudia</t>
   </si>
   <si>
-    <t>TC008</t>
-  </si>
-  <si>
     <t>KWI</t>
   </si>
   <si>
     <t>Kuwait</t>
-  </si>
-  <si>
-    <t>TC009</t>
   </si>
   <si>
     <t>MNL</t>
@@ -259,9 +232,6 @@
   </si>
   <si>
     <t>UK</t>
-  </si>
-  <si>
-    <t>TC010</t>
   </si>
   <si>
     <t>Singapore</t>
@@ -280,6 +250,9 @@
   </si>
   <si>
     <t>Language Code</t>
+  </si>
+  <si>
+    <t>TC001</t>
   </si>
   <si>
     <t>IRT</t>
@@ -1188,7 +1161,7 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.52344" defaultRowHeight="15"/>
@@ -1263,29 +1236,29 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="C2" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="D2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="8" t="s">
         <v>24</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>25</v>
       </c>
       <c r="F2" s="1">
         <v>45769</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>26</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>27</v>
       </c>
       <c r="I2" s="8">
         <v>1</v>
@@ -1306,48 +1279,48 @@
         <v>0</v>
       </c>
       <c r="O2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P2" s="8" t="b">
         <v>0</v>
       </c>
       <c r="Q2" t="s">
+        <v>28</v>
+      </c>
+      <c r="S2" t="s">
         <v>29</v>
-      </c>
-      <c r="S2" t="s">
-        <v>30</v>
       </c>
       <c r="T2" t="s">
         <v>15</v>
       </c>
       <c r="U2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
+      <c r="C3" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="D3" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="E3" s="8" t="s">
         <v>34</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>36</v>
       </c>
       <c r="F3" s="1">
         <v>45809</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>26</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>27</v>
       </c>
       <c r="I3" s="8">
         <v>1</v>
@@ -1368,48 +1341,48 @@
         <v>0</v>
       </c>
       <c r="O3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="P3" s="8" t="b">
         <v>0</v>
       </c>
       <c r="Q3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="S3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="T3" t="s">
         <v>15</v>
       </c>
       <c r="U3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="E4" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>43</v>
       </c>
       <c r="F4" s="1">
         <v>45728</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I4" s="8">
         <v>1</v>
@@ -1430,48 +1403,48 @@
         <v>1</v>
       </c>
       <c r="O4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="P4" s="8" t="b">
         <v>0</v>
       </c>
       <c r="Q4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="S4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="T4" t="s">
         <v>15</v>
       </c>
       <c r="U4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
-        <v>47</v>
+      <c r="A5">
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
         <v>22</v>
-      </c>
-      <c r="E5" t="s">
-        <v>23</v>
       </c>
       <c r="F5" s="1">
         <v>45752</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -1492,45 +1465,45 @@
         <v>0</v>
       </c>
       <c r="O5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="P5" t="b">
         <v>1</v>
       </c>
       <c r="Q5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="S5" t="s">
+        <v>48</v>
+      </c>
+      <c r="T5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" t="s">
         <v>52</v>
       </c>
-      <c r="T5" t="s">
+      <c r="E6" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D6" t="s">
-        <v>57</v>
-      </c>
-      <c r="E6" t="s">
-        <v>58</v>
       </c>
       <c r="F6" s="1">
         <v>45799</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="H6" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -1551,48 +1524,48 @@
         <v>1</v>
       </c>
       <c r="O6" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="P6" t="b">
         <v>0</v>
       </c>
       <c r="Q6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R6">
         <v>1</v>
       </c>
       <c r="S6" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="T6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s">
-        <v>63</v>
+      <c r="A7">
+        <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
         <v>22</v>
       </c>
-      <c r="C7" t="s">
-        <v>23</v>
-      </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F7" s="1">
         <v>45823</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="H7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -1613,45 +1586,45 @@
         <v>1</v>
       </c>
       <c r="O7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="P7" t="b">
         <v>1</v>
       </c>
       <c r="Q7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="S7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="T7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="s">
-        <v>65</v>
+      <c r="A8">
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C8" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F8" s="1">
         <v>45848</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="H8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="I8">
         <v>1</v>
@@ -1672,48 +1645,48 @@
         <v>0</v>
       </c>
       <c r="O8" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="P8" t="b">
         <v>0</v>
       </c>
       <c r="Q8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R8">
         <v>2</v>
       </c>
       <c r="S8" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="T8" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="s">
-        <v>71</v>
+      <c r="A9">
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C9" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="D9" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E9" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="F9" s="1">
         <v>45888</v>
       </c>
       <c r="G9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" t="s">
         <v>26</v>
-      </c>
-      <c r="H9" t="s">
-        <v>27</v>
       </c>
       <c r="I9">
         <v>1</v>
@@ -1734,45 +1707,45 @@
         <v>0</v>
       </c>
       <c r="O9" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="P9" t="b">
         <v>1</v>
       </c>
       <c r="Q9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="S9" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="T9" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="s">
-        <v>74</v>
+      <c r="A10">
+        <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
         <v>22</v>
       </c>
-      <c r="C10" t="s">
-        <v>23</v>
-      </c>
       <c r="D10" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="E10" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="F10" s="1">
         <v>45908</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="H10" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="I10">
         <v>1</v>
@@ -1793,45 +1766,45 @@
         <v>1</v>
       </c>
       <c r="O10" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="P10" t="b">
         <v>0</v>
       </c>
       <c r="Q10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="S10" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="T10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="s">
-        <v>78</v>
+      <c r="A11">
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="D11" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="E11" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="F11" s="1">
         <v>45951</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="H11" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="I11">
         <v>1</v>
@@ -1852,274 +1825,68 @@
         <v>0</v>
       </c>
       <c r="O11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="P11" t="b">
         <v>1</v>
       </c>
       <c r="Q11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="S11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="T11" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12"/>
-      <c r="B12"/>
-      <c r="C12"/>
-      <c r="D12"/>
-      <c r="E12"/>
       <c r="F12" s="1"/>
       <c r="G12" s="2"/>
-      <c r="H12"/>
-      <c r="I12"/>
-      <c r="J12"/>
-      <c r="K12"/>
-      <c r="L12"/>
-      <c r="M12"/>
-      <c r="N12"/>
-      <c r="O12"/>
-      <c r="P12"/>
-      <c r="Q12"/>
-      <c r="S12"/>
-      <c r="T12"/>
     </row>
     <row r="13">
-      <c r="A13"/>
-      <c r="B13"/>
-      <c r="C13"/>
-      <c r="D13"/>
-      <c r="E13"/>
       <c r="F13" s="1"/>
       <c r="G13" s="2"/>
-      <c r="H13"/>
-      <c r="I13"/>
-      <c r="J13"/>
-      <c r="K13"/>
-      <c r="L13"/>
-      <c r="M13"/>
-      <c r="N13"/>
-      <c r="P13"/>
-      <c r="Q13"/>
-      <c r="S13"/>
-      <c r="T13"/>
     </row>
     <row r="14">
-      <c r="A14"/>
-      <c r="B14"/>
-      <c r="C14"/>
-      <c r="D14"/>
-      <c r="E14"/>
       <c r="F14" s="1"/>
       <c r="G14" s="2"/>
-      <c r="H14"/>
-      <c r="I14"/>
-      <c r="J14"/>
-      <c r="K14"/>
-      <c r="L14"/>
-      <c r="M14"/>
-      <c r="N14"/>
-      <c r="O14"/>
-      <c r="P14"/>
-      <c r="Q14"/>
-      <c r="R14"/>
-      <c r="S14"/>
-      <c r="T14"/>
     </row>
     <row r="15">
-      <c r="A15"/>
-      <c r="B15"/>
-      <c r="C15"/>
-      <c r="D15"/>
-      <c r="E15"/>
       <c r="F15" s="1"/>
       <c r="G15" s="2"/>
-      <c r="H15"/>
-      <c r="I15"/>
-      <c r="J15"/>
-      <c r="K15"/>
-      <c r="L15"/>
-      <c r="M15"/>
-      <c r="N15"/>
-      <c r="O15"/>
-      <c r="P15"/>
-      <c r="Q15"/>
-      <c r="S15"/>
-      <c r="T15"/>
     </row>
     <row r="16">
-      <c r="A16"/>
-      <c r="B16"/>
-      <c r="C16"/>
-      <c r="D16"/>
-      <c r="E16"/>
       <c r="F16" s="1"/>
       <c r="G16" s="2"/>
-      <c r="H16"/>
-      <c r="I16"/>
-      <c r="J16"/>
-      <c r="K16"/>
-      <c r="L16"/>
-      <c r="M16"/>
-      <c r="N16"/>
-      <c r="O16"/>
-      <c r="P16"/>
-      <c r="Q16"/>
-      <c r="S16"/>
-      <c r="T16"/>
     </row>
     <row r="17">
-      <c r="A17"/>
-      <c r="B17"/>
-      <c r="C17"/>
-      <c r="D17"/>
-      <c r="E17"/>
       <c r="F17" s="1"/>
       <c r="G17" s="2"/>
-      <c r="H17"/>
-      <c r="I17"/>
-      <c r="J17"/>
-      <c r="K17"/>
-      <c r="L17"/>
-      <c r="M17"/>
-      <c r="N17"/>
-      <c r="O17"/>
-      <c r="P17"/>
-      <c r="Q17"/>
-      <c r="R17"/>
-      <c r="S17"/>
-      <c r="T17"/>
     </row>
     <row r="18">
-      <c r="A18"/>
-      <c r="B18"/>
-      <c r="C18"/>
-      <c r="D18"/>
-      <c r="E18"/>
       <c r="F18" s="1"/>
       <c r="G18" s="2"/>
-      <c r="H18"/>
-      <c r="I18"/>
-      <c r="J18"/>
-      <c r="K18"/>
-      <c r="L18"/>
-      <c r="M18"/>
-      <c r="N18"/>
-      <c r="P18"/>
-      <c r="Q18"/>
-      <c r="S18"/>
-      <c r="T18"/>
     </row>
     <row r="19">
-      <c r="A19"/>
-      <c r="B19"/>
-      <c r="C19"/>
-      <c r="D19"/>
-      <c r="E19"/>
       <c r="F19" s="1"/>
       <c r="G19" s="2"/>
-      <c r="H19"/>
-      <c r="I19"/>
-      <c r="J19"/>
-      <c r="K19"/>
-      <c r="L19"/>
-      <c r="M19"/>
-      <c r="N19"/>
-      <c r="P19"/>
-      <c r="Q19"/>
-      <c r="R19"/>
-      <c r="S19"/>
-      <c r="T19"/>
     </row>
     <row r="20">
-      <c r="A20"/>
-      <c r="B20"/>
-      <c r="C20"/>
-      <c r="D20"/>
-      <c r="E20"/>
       <c r="F20" s="1"/>
       <c r="G20" s="2"/>
-      <c r="H20"/>
-      <c r="I20"/>
-      <c r="J20"/>
-      <c r="K20"/>
-      <c r="L20"/>
-      <c r="M20"/>
-      <c r="N20"/>
-      <c r="P20"/>
-      <c r="Q20"/>
-      <c r="R20"/>
-      <c r="S20"/>
-      <c r="T20"/>
     </row>
     <row r="21">
-      <c r="A21"/>
-      <c r="B21"/>
-      <c r="C21"/>
-      <c r="D21"/>
-      <c r="E21"/>
       <c r="F21" s="1"/>
       <c r="G21" s="2"/>
-      <c r="H21"/>
-      <c r="I21"/>
-      <c r="J21"/>
-      <c r="K21"/>
-      <c r="L21"/>
-      <c r="M21"/>
-      <c r="N21"/>
-      <c r="O21"/>
-      <c r="P21"/>
-      <c r="Q21"/>
-      <c r="R21"/>
-      <c r="S21"/>
-      <c r="T21"/>
     </row>
     <row r="22">
-      <c r="A22"/>
-      <c r="B22"/>
-      <c r="C22"/>
-      <c r="D22"/>
-      <c r="E22"/>
       <c r="F22" s="1"/>
       <c r="G22" s="2"/>
-      <c r="H22"/>
-      <c r="I22"/>
-      <c r="J22"/>
-      <c r="K22"/>
-      <c r="L22"/>
-      <c r="M22"/>
-      <c r="N22"/>
-      <c r="O22"/>
-      <c r="P22"/>
-      <c r="Q22"/>
-      <c r="R22"/>
-      <c r="S22"/>
-      <c r="T22"/>
     </row>
     <row r="23">
-      <c r="A23"/>
-      <c r="B23"/>
-      <c r="C23"/>
-      <c r="D23"/>
-      <c r="E23"/>
       <c r="F23" s="1"/>
       <c r="G23" s="2"/>
-      <c r="H23"/>
-      <c r="I23"/>
-      <c r="J23"/>
-      <c r="K23"/>
-      <c r="L23"/>
-      <c r="M23"/>
-      <c r="N23"/>
-      <c r="O23"/>
-      <c r="P23"/>
-      <c r="Q23"/>
-      <c r="S23"/>
-      <c r="T23"/>
     </row>
   </sheetData>
   <pageSetup r:id="rId1" orientation="portrait"/>
@@ -2154,7 +1921,7 @@
         <v>5</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>7</v>
@@ -2178,10 +1945,10 @@
         <v>13</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="O1" s="4" t="s">
         <v>6</v>
@@ -2204,13 +1971,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>22</v>
-      </c>
       <c r="C2" s="8" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D2" s="10">
         <v>45699</v>
@@ -2219,7 +1986,7 @@
         <v>45704</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G2" s="8">
         <v>2</v>
@@ -2240,16 +2007,16 @@
         <v>0</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="O2" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P2" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="T2" t="s">
         <v>15</v>
@@ -2310,34 +2077,34 @@
         <v>16</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="M1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="T1" s="4" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="U1" s="4" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="V1" s="7" t="s">
         <v>15</v>
@@ -2354,16 +2121,16 @@
     </row>
     <row r="2" ht="14.4">
       <c r="A2" s="8" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" s="11">
         <v>45632</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E2" s="8">
         <v>1</v>
@@ -2384,46 +2151,46 @@
         <v>0</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O2" s="8" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="P2" s="11">
         <v>45639</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R2" s="8" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="S2" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="T2" s="11">
         <v>45641</v>
       </c>
       <c r="U2" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="V2" s="8" t="b">
         <v>0</v>
       </c>
       <c r="W2" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="X2" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="Y2" t="s">
         <v>15</v>
@@ -2467,64 +2234,64 @@
         <v>7</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="S1" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="V1" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>100</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="U1" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="V1" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="W1" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="X1" s="4" t="s">
-        <v>109</v>
       </c>
       <c r="Y1" s="4" t="s">
         <v>8</v>
@@ -2548,7 +2315,7 @@
         <v>16</v>
       </c>
       <c r="AF1" s="4" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="AG1" s="4" t="s">
         <v>6</v>
@@ -2559,76 +2326,76 @@
     </row>
     <row r="2" ht="14.4">
       <c r="A2" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C2" s="11">
         <v>45602</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G2" s="11">
         <v>45610</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="K2" s="11">
         <v>45611</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O2" s="11">
         <v>45614</v>
       </c>
       <c r="P2" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="R2" s="8" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="S2" s="11">
         <v>45621</v>
       </c>
       <c r="T2" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="U2" s="8" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="V2" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="W2" s="11">
         <v>45623</v>
       </c>
       <c r="X2" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Y2" s="8">
         <v>3</v>
@@ -2649,13 +2416,13 @@
         <v>0</v>
       </c>
       <c r="AE2" s="8" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="AF2" s="8" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="AG2" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="AH2" s="8" t="b">
         <v>0</v>
@@ -2684,7 +2451,7 @@
   <sheetData>
     <row r="1" ht="15" customHeight="1">
       <c r="A1" s="13" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -2712,25 +2479,25 @@
     </row>
     <row r="2" ht="15" customHeight="1">
       <c r="A2" s="15" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
@@ -2752,7 +2519,7 @@
     </row>
     <row r="3" ht="15" customHeight="1">
       <c r="A3" s="14" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="B3" s="17">
         <v>4005550000000000</v>
@@ -2788,7 +2555,7 @@
     </row>
     <row r="4" ht="15" customHeight="1">
       <c r="A4" s="14" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="B4" s="17">
         <v>5123456789012340</v>
@@ -2824,7 +2591,7 @@
     </row>
     <row r="5" ht="15" customHeight="1">
       <c r="A5" s="14" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="B5" s="17">
         <v>345678901234564</v>
@@ -2886,7 +2653,7 @@
     </row>
     <row r="7" ht="15" customHeight="1">
       <c r="A7" s="13" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
@@ -2914,25 +2681,25 @@
     </row>
     <row r="8" ht="15" customHeight="1">
       <c r="A8" s="15" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C8" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="F8" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="D8" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>123</v>
-      </c>
       <c r="G8" s="15" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
@@ -2954,7 +2721,7 @@
     </row>
     <row r="9" ht="15" customHeight="1">
       <c r="A9" s="14" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B9" s="17">
         <v>5531886652142950</v>
@@ -2994,7 +2761,7 @@
     </row>
     <row r="10" ht="15" customHeight="1">
       <c r="A10" s="14" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B10" s="17">
         <v>4187427415564240</v>
@@ -3060,7 +2827,7 @@
     </row>
     <row r="12" ht="15" customHeight="1">
       <c r="A12" s="13" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="B12" s="13"/>
       <c r="C12" s="13"/>
@@ -3088,22 +2855,22 @@
     </row>
     <row r="13" ht="15" customHeight="1">
       <c r="A13" s="15" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
@@ -3133,7 +2900,7 @@
         <v>12</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="E14" s="14">
         <v>0</v>
@@ -3169,7 +2936,7 @@
         <v>12</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="E15" s="14">
         <v>0</v>
@@ -3205,7 +2972,7 @@
         <v>12</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="E16" s="14">
         <v>0</v>
@@ -3241,7 +3008,7 @@
         <v>12</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="E17" s="14">
         <v>0</v>
@@ -3277,7 +3044,7 @@
         <v>12</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="E18" s="14">
         <v>0</v>
@@ -3306,7 +3073,7 @@
     </row>
     <row r="19" ht="15" customHeight="1">
       <c r="A19" s="14" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="B19" s="18">
         <v>4000000000000010</v>
@@ -3315,16 +3082,16 @@
         <v>12</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="E19" s="14">
         <v>0</v>
       </c>
       <c r="F19" s="14" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="H19" s="14"/>
       <c r="I19" s="14"/>
@@ -3353,7 +3120,7 @@
         <v>12</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="E20" s="14">
         <v>0</v>
@@ -3362,7 +3129,7 @@
         <v>123</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
@@ -3410,7 +3177,7 @@
     </row>
     <row r="22" ht="15" customHeight="1">
       <c r="A22" s="13" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="B22" s="13"/>
       <c r="C22" s="13"/>
@@ -3438,25 +3205,25 @@
     </row>
     <row r="23" ht="15" customHeight="1">
       <c r="A23" s="15" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C23" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="F23" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="D23" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="F23" s="15" t="s">
-        <v>123</v>
-      </c>
       <c r="G23" s="15" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="H23" s="14"/>
       <c r="I23" s="14"/>
@@ -3478,7 +3245,7 @@
     </row>
     <row r="24" ht="15" customHeight="1">
       <c r="A24" s="14" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B24" s="17">
         <v>5577810000000000</v>
@@ -3544,7 +3311,7 @@
     </row>
     <row r="26" ht="15" customHeight="1">
       <c r="A26" s="13" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
@@ -3572,19 +3339,19 @@
     </row>
     <row r="27" ht="15" customHeight="1">
       <c r="A27" s="15" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
@@ -3608,7 +3375,7 @@
     </row>
     <row r="28" ht="15" customHeight="1">
       <c r="A28" s="14" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B28" s="17">
         <v>4242424242424240</v>
@@ -3670,7 +3437,7 @@
     </row>
     <row r="30" ht="15" customHeight="1">
       <c r="A30" s="13" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="B30" s="13"/>
       <c r="C30" s="13"/>
@@ -3698,19 +3465,19 @@
     </row>
     <row r="31" ht="15" customHeight="1">
       <c r="A31" s="15" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="F31" s="14"/>
       <c r="G31" s="14"/>
@@ -3734,16 +3501,16 @@
     </row>
     <row r="32" ht="15" customHeight="1">
       <c r="A32" s="14" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B32" s="17">
         <v>5200000000000000</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="E32" s="14">
         <v>123</v>
@@ -3796,7 +3563,7 @@
     </row>
     <row r="34" ht="15" customHeight="1">
       <c r="A34" s="13" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="B34" s="13"/>
       <c r="C34" s="13"/>
@@ -3824,19 +3591,19 @@
     </row>
     <row r="35" ht="15" customHeight="1">
       <c r="A35" s="15" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="E35" s="15" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="F35" s="14"/>
       <c r="G35" s="14"/>
@@ -3860,7 +3627,7 @@
     </row>
     <row r="36" ht="15" customHeight="1">
       <c r="A36" s="14" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B36" s="17">
         <v>5204730000002510</v>
@@ -3896,7 +3663,7 @@
     </row>
     <row r="37" ht="15" customHeight="1">
       <c r="A37" s="14" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B37" s="17">
         <v>4111111111111110</v>
@@ -3958,7 +3725,7 @@
     </row>
     <row r="39" ht="15" customHeight="1">
       <c r="A39" s="13" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="B39" s="13"/>
       <c r="C39" s="13"/>
@@ -3986,25 +3753,25 @@
     </row>
     <row r="40" ht="15" customHeight="1">
       <c r="A40" s="15" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="D40" s="15" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="E40" s="15" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="F40" s="15" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="G40" s="15" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="H40" s="14"/>
       <c r="I40" s="14"/>
@@ -4026,19 +3793,19 @@
     </row>
     <row r="41" ht="15" customHeight="1">
       <c r="A41" s="14" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B41" s="17">
         <v>4111111111111110</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="D41" s="14" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="E41" s="14" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="F41" s="14">
         <v>8888</v>
@@ -4092,7 +3859,7 @@
     </row>
     <row r="43" ht="15" customHeight="1">
       <c r="A43" s="13" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B43" s="13"/>
       <c r="C43" s="13"/>
@@ -4120,19 +3887,19 @@
     </row>
     <row r="44" ht="15" customHeight="1">
       <c r="A44" s="15" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="D44" s="15" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="E44" s="15" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="F44" s="14"/>
       <c r="G44" s="14"/>
@@ -4156,16 +3923,16 @@
     </row>
     <row r="45" ht="15" customHeight="1">
       <c r="A45" s="14" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B45" s="17">
         <v>4000000000000000</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="D45" s="14" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="E45" s="14">
         <v>123</v>
@@ -4270,7 +4037,7 @@
     </row>
     <row r="49" ht="15" customHeight="1">
       <c r="A49" s="13" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="B49" s="13"/>
       <c r="C49" s="13"/>
@@ -4298,19 +4065,19 @@
     </row>
     <row r="50" ht="15" customHeight="1">
       <c r="A50" s="15" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B50" s="16" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="D50" s="15" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="E50" s="15" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="F50" s="14"/>
       <c r="G50" s="14"/>
@@ -4334,7 +4101,7 @@
     </row>
     <row r="51" ht="15" customHeight="1">
       <c r="A51" s="14" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B51" s="17">
         <v>4000000000001090</v>
@@ -4404,7 +4171,7 @@
     </row>
     <row r="53" ht="15" customHeight="1">
       <c r="A53" s="14" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B53" s="17">
         <v>5200000000001090</v>
@@ -4552,7 +4319,7 @@
     </row>
     <row r="58" ht="15" customHeight="1">
       <c r="A58" s="13" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="B58" s="13"/>
       <c r="C58" s="13"/>
@@ -4658,7 +4425,7 @@
     </row>
     <row r="62" ht="15" customHeight="1">
       <c r="A62" s="13" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B62" s="13"/>
       <c r="C62" s="13"/>
@@ -4686,25 +4453,25 @@
     </row>
     <row r="63" ht="15" customHeight="1">
       <c r="A63" s="15" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B63" s="16" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C63" s="15" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="D63" s="15" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="E63" s="15" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="F63" s="15" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="G63" s="15" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="H63" s="14"/>
       <c r="I63" s="14"/>
@@ -4740,7 +4507,7 @@
       </c>
       <c r="F64" s="14"/>
       <c r="G64" s="14" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="H64" s="14"/>
       <c r="I64" s="14"/>
@@ -4814,7 +4581,7 @@
     </row>
     <row r="67" ht="15" customHeight="1">
       <c r="A67" s="13" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="B67" s="13"/>
       <c r="C67" s="13"/>
@@ -4870,7 +4637,7 @@
     </row>
     <row r="69" ht="15" customHeight="1">
       <c r="A69" s="14" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="B69" s="17"/>
       <c r="C69" s="14"/>
@@ -4980,7 +4747,7 @@
     </row>
     <row r="73" ht="15" customHeight="1">
       <c r="A73" s="20" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="B73" s="20"/>
       <c r="C73" s="20"/>
@@ -5008,19 +4775,19 @@
     </row>
     <row r="74" ht="15" customHeight="1">
       <c r="A74" s="14" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B74" s="17" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="C74" s="14" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="D74" s="14" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="E74" s="14" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="F74" s="14"/>
       <c r="G74" s="14"/>
@@ -5044,13 +4811,13 @@
     </row>
     <row r="75" ht="15" customHeight="1">
       <c r="A75" s="14" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="B75" s="17" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="C75" s="14" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="D75" s="14">
         <v>47543</v>
@@ -5106,7 +4873,7 @@
     </row>
     <row r="77" ht="15" customHeight="1">
       <c r="A77" s="14" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B77" s="17"/>
       <c r="C77" s="14"/>
@@ -5134,19 +4901,19 @@
     </row>
     <row r="78" ht="15" customHeight="1">
       <c r="A78" s="14" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B78" s="17" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="C78" s="14" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="D78" s="14" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="E78" s="14" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="F78" s="14"/>
       <c r="G78" s="14"/>
@@ -5170,13 +4937,13 @@
     </row>
     <row r="79" ht="15" customHeight="1">
       <c r="A79" s="14" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="B79" s="17" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C79" s="14" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="D79" s="14">
         <v>47543</v>
@@ -5232,7 +4999,7 @@
     </row>
     <row r="81" ht="15" customHeight="1">
       <c r="A81" s="21" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="B81" s="21"/>
       <c r="C81" s="21"/>
@@ -5260,10 +5027,10 @@
     </row>
     <row r="82" ht="15" customHeight="1">
       <c r="A82" s="14" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="B82" s="17" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C82" s="14"/>
       <c r="D82" s="14"/>
@@ -5290,7 +5057,7 @@
     </row>
     <row r="83" ht="15" customHeight="1">
       <c r="A83" s="14" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B83" s="17">
         <v>5123450000000000</v>
@@ -5404,7 +5171,7 @@
     </row>
     <row r="87" ht="15" customHeight="1">
       <c r="A87" s="14" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B87" s="17">
         <v>4508750015741010</v>
@@ -5462,7 +5229,7 @@
     </row>
     <row r="89" ht="15" customHeight="1">
       <c r="A89" s="22" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B89" s="22"/>
       <c r="C89" s="22"/>
@@ -5490,7 +5257,7 @@
     </row>
     <row r="90" ht="15" customHeight="1">
       <c r="A90" s="14" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="B90" s="17"/>
       <c r="C90" s="14"/>
@@ -5570,7 +5337,7 @@
     </row>
     <row r="93" ht="15" customHeight="1">
       <c r="A93" s="22" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="B93" s="22"/>
       <c r="C93" s="22"/>
@@ -5598,22 +5365,22 @@
     </row>
     <row r="94" ht="15" customHeight="1">
       <c r="A94" s="14" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B94" s="17" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C94" s="14" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="D94" s="14" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="E94" s="14" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="F94" s="14" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="G94" s="14"/>
       <c r="H94" s="14"/>
@@ -5636,7 +5403,7 @@
     </row>
     <row r="95" ht="15" customHeight="1">
       <c r="A95" s="14" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="B95" s="17">
         <v>11933</v>
@@ -5651,7 +5418,7 @@
         <v>12345</v>
       </c>
       <c r="F95" s="14" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="G95" s="14"/>
       <c r="H95" s="14"/>
@@ -5674,7 +5441,7 @@
     </row>
     <row r="96" ht="15" customHeight="1">
       <c r="A96" s="14" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="B96" s="17">
         <v>11933</v>
@@ -5689,7 +5456,7 @@
         <v>12345</v>
       </c>
       <c r="F96" s="14" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="G96" s="14"/>
       <c r="H96" s="14"/>
@@ -5712,7 +5479,7 @@
     </row>
     <row r="97" ht="15" customHeight="1">
       <c r="A97" s="14" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="B97" s="17">
         <v>45596</v>
@@ -5727,7 +5494,7 @@
         <v>12345</v>
       </c>
       <c r="F97" s="14" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="G97" s="14"/>
       <c r="H97" s="14"/>
@@ -5776,7 +5543,7 @@
     </row>
     <row r="99" ht="15" customHeight="1">
       <c r="A99" s="22" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="B99" s="22"/>
       <c r="C99" s="22"/>
@@ -5914,7 +5681,7 @@
     </row>
     <row r="104" ht="15" customHeight="1">
       <c r="A104" s="22" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="B104" s="22"/>
       <c r="C104" s="22"/>
@@ -5942,7 +5709,7 @@
     </row>
     <row r="105" ht="15" customHeight="1">
       <c r="A105" s="14" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="B105" s="17"/>
       <c r="C105" s="14"/>
@@ -5970,23 +5737,23 @@
     </row>
     <row r="106" ht="15" customHeight="1">
       <c r="A106" s="14" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="B106" s="17" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C106" s="14" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="D106" s="14" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="E106" s="14" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="F106" s="14"/>
       <c r="G106" s="14" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="H106" s="14"/>
       <c r="I106" s="14"/>
@@ -6008,7 +5775,7 @@
     </row>
     <row r="107" ht="15" customHeight="1">
       <c r="A107" s="14" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="B107" s="17">
         <v>8888880000000000</v>
@@ -6020,11 +5787,11 @@
         <v>1234</v>
       </c>
       <c r="E107" s="14" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="F107" s="14"/>
       <c r="G107" s="14" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="H107" s="14"/>
       <c r="I107" s="14"/>
@@ -6046,7 +5813,7 @@
     </row>
     <row r="108" ht="15" customHeight="1">
       <c r="A108" s="14" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="B108" s="17">
         <v>8888880000000000</v>
@@ -6058,7 +5825,7 @@
         <v>1234</v>
       </c>
       <c r="E108" s="14" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="F108" s="14"/>
       <c r="G108" s="19">
@@ -6136,7 +5903,7 @@
     </row>
     <row r="111" ht="15" customHeight="1">
       <c r="A111" s="14" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="B111" s="17"/>
       <c r="C111" s="14"/>
@@ -6164,13 +5931,13 @@
     </row>
     <row r="112" ht="15" customHeight="1">
       <c r="A112" s="14" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="B112" s="17" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C112" s="14" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="D112" s="14"/>
       <c r="E112" s="14"/>
@@ -6196,13 +5963,13 @@
     </row>
     <row r="113" ht="15" customHeight="1">
       <c r="A113" s="14" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="B113" s="17">
         <v>5123450000000000</v>
       </c>
       <c r="C113" s="14" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="D113" s="14"/>
       <c r="E113" s="14"/>
@@ -6228,13 +5995,13 @@
     </row>
     <row r="114" ht="15" customHeight="1">
       <c r="A114" s="14" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="B114" s="17">
         <v>5111111111111110</v>
       </c>
       <c r="C114" s="14" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="D114" s="14"/>
       <c r="E114" s="14"/>
@@ -6260,13 +6027,13 @@
     </row>
     <row r="115" ht="15" customHeight="1">
       <c r="A115" s="14" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="B115" s="17">
         <v>4508750015741010</v>
       </c>
       <c r="C115" s="14" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="D115" s="14"/>
       <c r="E115" s="14"/>
@@ -6292,13 +6059,13 @@
     </row>
     <row r="116" ht="15" customHeight="1">
       <c r="A116" s="14" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="B116" s="17">
         <v>4012000033330020</v>
       </c>
       <c r="C116" s="14" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="D116" s="14"/>
       <c r="E116" s="14"/>
@@ -6324,7 +6091,7 @@
     </row>
     <row r="117" ht="15" customHeight="1">
       <c r="A117" s="22" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="B117" s="22"/>
       <c r="C117" s="22"/>
@@ -6352,7 +6119,7 @@
     </row>
     <row r="118" ht="15" customHeight="1">
       <c r="A118" s="14" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="B118" s="17"/>
       <c r="C118" s="14"/>
@@ -6380,7 +6147,7 @@
     </row>
     <row r="119" ht="15" customHeight="1">
       <c r="A119" s="14" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="B119" s="17"/>
       <c r="C119" s="14"/>
@@ -6434,7 +6201,7 @@
     </row>
     <row r="121" ht="15" customHeight="1">
       <c r="A121" s="22" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="B121" s="22"/>
       <c r="C121" s="22"/>
@@ -6462,7 +6229,7 @@
     </row>
     <row r="122" ht="15" customHeight="1">
       <c r="A122" s="14" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="B122" s="17"/>
       <c r="C122" s="14"/>
@@ -6490,7 +6257,7 @@
     </row>
     <row r="123" ht="15" customHeight="1">
       <c r="A123" s="14" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="B123" s="17"/>
       <c r="C123" s="14"/>
@@ -6518,7 +6285,7 @@
     </row>
     <row r="124" ht="15" customHeight="1">
       <c r="A124" s="14" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="B124" s="17"/>
       <c r="C124" s="14"/>
@@ -29519,93 +29286,93 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D1" t="s">
+        <v>192</v>
+      </c>
+      <c r="E1" t="s">
+        <v>193</v>
+      </c>
+      <c r="F1" t="s">
+        <v>194</v>
+      </c>
+      <c r="G1" t="s">
+        <v>195</v>
+      </c>
+      <c r="H1" t="s">
+        <v>196</v>
+      </c>
+      <c r="I1" t="s">
+        <v>197</v>
+      </c>
+      <c r="J1" t="s">
         <v>198</v>
       </c>
-      <c r="B1" t="s">
+      <c r="K1" t="s">
         <v>199</v>
       </c>
-      <c r="C1" t="s">
+      <c r="L1" t="s">
         <v>200</v>
       </c>
-      <c r="D1" t="s">
+      <c r="M1" t="s">
         <v>201</v>
       </c>
-      <c r="E1" t="s">
+      <c r="N1" t="s">
         <v>202</v>
       </c>
-      <c r="F1" t="s">
+      <c r="O1" t="s">
         <v>203</v>
       </c>
-      <c r="G1" t="s">
+      <c r="P1" t="s">
         <v>204</v>
       </c>
-      <c r="H1" t="s">
+      <c r="Q1" s="23" t="s">
         <v>205</v>
-      </c>
-      <c r="I1" t="s">
-        <v>206</v>
-      </c>
-      <c r="J1" t="s">
-        <v>207</v>
-      </c>
-      <c r="K1" t="s">
-        <v>208</v>
-      </c>
-      <c r="L1" t="s">
-        <v>209</v>
-      </c>
-      <c r="M1" t="s">
-        <v>210</v>
-      </c>
-      <c r="N1" t="s">
-        <v>211</v>
-      </c>
-      <c r="O1" t="s">
-        <v>212</v>
-      </c>
-      <c r="P1" t="s">
-        <v>213</v>
-      </c>
-      <c r="Q1" s="23" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="B2" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="C2" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="D2">
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="F2">
         <v>2014</v>
       </c>
       <c r="G2" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="H2" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="I2" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="J2" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="K2">
         <v>20</v>
       </c>
       <c r="L2" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="M2">
         <v>2022</v>
@@ -29614,7 +29381,7 @@
         <v>20</v>
       </c>
       <c r="O2" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="P2">
         <v>2033</v>
@@ -29625,40 +29392,40 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="B3" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="C3" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="D3">
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="F3">
         <v>2014</v>
       </c>
       <c r="G3" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="H3" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="I3" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="J3" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="K3">
         <v>20</v>
       </c>
       <c r="L3" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="M3">
         <v>2022</v>
@@ -29667,7 +29434,7 @@
         <v>21</v>
       </c>
       <c r="O3" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="P3">
         <v>2033</v>
@@ -29675,37 +29442,37 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="B4" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="C4" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="D4">
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="F4">
         <v>2014</v>
       </c>
       <c r="H4" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="I4" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="J4" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="K4">
         <v>20</v>
       </c>
       <c r="L4" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="M4">
         <v>2022</v>
@@ -29714,7 +29481,7 @@
         <v>22</v>
       </c>
       <c r="O4" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="P4">
         <v>2033</v>
@@ -29722,37 +29489,37 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="B5" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="C5" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="D5">
         <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="F5">
         <v>2014</v>
       </c>
       <c r="H5" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="I5" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="J5" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="K5">
         <v>20</v>
       </c>
       <c r="L5" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="M5">
         <v>2022</v>
@@ -29761,7 +29528,7 @@
         <v>23</v>
       </c>
       <c r="O5" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="P5">
         <v>2033</v>
@@ -29786,90 +29553,90 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D1" t="s">
+        <v>192</v>
+      </c>
+      <c r="E1" t="s">
+        <v>193</v>
+      </c>
+      <c r="F1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G1" t="s">
+        <v>194</v>
+      </c>
+      <c r="H1" t="s">
+        <v>196</v>
+      </c>
+      <c r="I1" t="s">
+        <v>197</v>
+      </c>
+      <c r="J1" t="s">
         <v>198</v>
       </c>
-      <c r="B1" t="s">
+      <c r="K1" t="s">
         <v>199</v>
       </c>
-      <c r="C1" t="s">
+      <c r="L1" t="s">
         <v>200</v>
       </c>
-      <c r="D1" t="s">
+      <c r="M1" t="s">
         <v>201</v>
       </c>
-      <c r="E1" t="s">
+      <c r="N1" t="s">
         <v>202</v>
       </c>
-      <c r="F1" t="s">
+      <c r="O1" t="s">
+        <v>203</v>
+      </c>
+      <c r="P1" t="s">
         <v>204</v>
-      </c>
-      <c r="G1" t="s">
-        <v>203</v>
-      </c>
-      <c r="H1" t="s">
-        <v>205</v>
-      </c>
-      <c r="I1" t="s">
-        <v>206</v>
-      </c>
-      <c r="J1" t="s">
-        <v>207</v>
-      </c>
-      <c r="K1" t="s">
-        <v>208</v>
-      </c>
-      <c r="L1" t="s">
-        <v>209</v>
-      </c>
-      <c r="M1" t="s">
-        <v>210</v>
-      </c>
-      <c r="N1" t="s">
-        <v>211</v>
-      </c>
-      <c r="O1" t="s">
-        <v>212</v>
-      </c>
-      <c r="P1" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="B2" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="C2" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="D2">
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="F2" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="G2">
         <v>2023</v>
       </c>
       <c r="H2" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="I2" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="J2" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="K2">
         <v>20</v>
       </c>
       <c r="L2" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="M2">
         <v>2024</v>
@@ -29878,7 +29645,7 @@
         <v>20</v>
       </c>
       <c r="O2" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="P2">
         <v>2034</v>
@@ -29886,40 +29653,40 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="B3" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="C3" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="D3">
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="F3" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="G3">
         <v>2023</v>
       </c>
       <c r="H3" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="I3" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="J3" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="K3">
         <v>20</v>
       </c>
       <c r="L3" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="M3">
         <v>2024</v>
@@ -29928,7 +29695,7 @@
         <v>21</v>
       </c>
       <c r="O3" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="P3">
         <v>2034</v>
@@ -29936,37 +29703,37 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="B4" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="C4" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="D4">
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="G4">
         <v>2023</v>
       </c>
       <c r="H4" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="I4" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="J4" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="K4">
         <v>20</v>
       </c>
       <c r="L4" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="M4">
         <v>2024</v>
@@ -29975,7 +29742,7 @@
         <v>22</v>
       </c>
       <c r="O4" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="P4">
         <v>2034</v>
@@ -29983,37 +29750,37 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="B5" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="C5" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="D5">
         <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="G5">
         <v>2023</v>
       </c>
       <c r="H5" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="I5" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="J5" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="K5">
         <v>20</v>
       </c>
       <c r="L5" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="M5">
         <v>2024</v>
@@ -30022,7 +29789,7 @@
         <v>23</v>
       </c>
       <c r="O5" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="P5">
         <v>2034</v>
@@ -30047,93 +29814,93 @@
   <sheetData>
     <row r="1" ht="30">
       <c r="A1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="C1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D1" t="s">
+        <v>192</v>
+      </c>
+      <c r="E1" t="s">
+        <v>193</v>
+      </c>
+      <c r="F1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G1" t="s">
+        <v>194</v>
+      </c>
+      <c r="H1" t="s">
+        <v>196</v>
+      </c>
+      <c r="I1" t="s">
+        <v>197</v>
+      </c>
+      <c r="J1" t="s">
         <v>198</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="K1" t="s">
         <v>199</v>
       </c>
-      <c r="C1" t="s">
+      <c r="L1" t="s">
         <v>200</v>
       </c>
-      <c r="D1" t="s">
+      <c r="M1" t="s">
         <v>201</v>
       </c>
-      <c r="E1" t="s">
+      <c r="N1" t="s">
         <v>202</v>
       </c>
-      <c r="F1" t="s">
+      <c r="O1" t="s">
+        <v>203</v>
+      </c>
+      <c r="P1" t="s">
         <v>204</v>
       </c>
-      <c r="G1" t="s">
-        <v>203</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="Q1" s="23" t="s">
         <v>205</v>
-      </c>
-      <c r="I1" t="s">
-        <v>206</v>
-      </c>
-      <c r="J1" t="s">
-        <v>207</v>
-      </c>
-      <c r="K1" t="s">
-        <v>208</v>
-      </c>
-      <c r="L1" t="s">
-        <v>209</v>
-      </c>
-      <c r="M1" t="s">
-        <v>210</v>
-      </c>
-      <c r="N1" t="s">
-        <v>211</v>
-      </c>
-      <c r="O1" t="s">
-        <v>212</v>
-      </c>
-      <c r="P1" t="s">
-        <v>213</v>
-      </c>
-      <c r="Q1" s="23" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="C2" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="D2">
         <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="F2" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="G2">
         <v>1995</v>
       </c>
       <c r="H2" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="I2" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="J2" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="K2">
         <v>20</v>
       </c>
       <c r="L2" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="M2">
         <v>2022</v>
@@ -30142,7 +29909,7 @@
         <v>20</v>
       </c>
       <c r="O2" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="P2">
         <v>2033</v>
@@ -30153,40 +29920,40 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="C3" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="D3">
         <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="F3" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="G3">
         <v>1996</v>
       </c>
       <c r="H3" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="I3" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="J3" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="K3">
         <v>20</v>
       </c>
       <c r="L3" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="M3">
         <v>2022</v>
@@ -30195,7 +29962,7 @@
         <v>21</v>
       </c>
       <c r="O3" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="P3">
         <v>2034</v>
@@ -30203,40 +29970,40 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="B4" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="C4" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="D4">
         <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="F4" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="G4">
         <v>1997</v>
       </c>
       <c r="H4" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="I4" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="J4" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="K4">
         <v>20</v>
       </c>
       <c r="L4" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="M4">
         <v>2022</v>
@@ -30245,7 +30012,7 @@
         <v>22</v>
       </c>
       <c r="O4" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="P4">
         <v>2035</v>
@@ -30253,37 +30020,37 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="B5" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="C5" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="D5">
         <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="G5">
         <v>1998</v>
       </c>
       <c r="H5" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="I5" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="J5" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="K5">
         <v>20</v>
       </c>
       <c r="L5" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="M5">
         <v>2022</v>
@@ -30292,7 +30059,7 @@
         <v>23</v>
       </c>
       <c r="O5" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="P5">
         <v>2033</v>
@@ -30300,37 +30067,37 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="B6" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="C6" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="D6">
         <v>23</v>
       </c>
       <c r="E6" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="G6">
         <v>1998</v>
       </c>
       <c r="H6" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="I6" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="J6" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="K6">
         <v>20</v>
       </c>
       <c r="L6" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="M6">
         <v>2022</v>
@@ -30339,7 +30106,7 @@
         <v>23</v>
       </c>
       <c r="O6" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="P6">
         <v>2033</v>

</xml_diff>